<commit_message>
feat: :sparkles: Pasamos la unidad, SIU
</commit_message>
<xml_diff>
--- a/ArchivosExcel/Indeed-Programador.xlsx
+++ b/ArchivosExcel/Indeed-Programador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Programador Web</t>
+          <t>Monitorista</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ryscode</t>
+          <t>SISTEMAS DE SEGURIDAD PRIVADA ARGOS S.A. DE C.V.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$16,000 a $18,000 por mes</t>
+          <t>$10,000 por mes</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,12 +500,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Programador .NET</t>
+          <t>Desarrollador Web</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ryscode</t>
+          <t>SISTEMAS DE SEGURIDAD PRIVADA ARGOS S.A. DE C.V.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$12,000 a $18,000 por mes</t>
+          <t>$13,000 a $15,000 por mes</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -532,12 +532,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Programador para integración</t>
+          <t>ESPECILISTA DENTAL para trabajar en Torreón ( ingreso mínimo asegurado)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Grupo Industriales Ercam</t>
+          <t>LOS DENTISTAS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Desde $14,000 por mes</t>
+          <t>$25,000 a $50,000 por mes</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -556,6 +556,390 @@
         </is>
       </c>
       <c r="F4" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Supervisor de Atención a Clientes</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Paquetexpress</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$14,900 por mes</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Postulación vía Indeed</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ANALISTA GASTOS DE VIAJE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Grupo LALA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ASESOR DE SERVICIO AUTOMOTRIZ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GRUPO ALAMEDA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$2,000 a $3,500 por semana</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Postulación vía Indeed</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MESERO/VENDEDOR</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PUCCINO´S - Restaurante-Bar Italiano</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Tiempo completo</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Postulación vía Indeed</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Auxiliar Administrativo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Constructora Cayarga, S.A de C.V.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>27110, Residencial los Llanos, Coah.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Recepcionista Español - Dirección Comercial</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Peñoles</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$10,000 a $12,000 por mes</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Postulación vía Indeed</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CAJERO (A)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SEPSA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>27000, Torreón Centro, Coah.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SUPERVISOR ALMACEN</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Grupo Modelo</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Asistente Administrativo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Easy Way Products</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>27280, Eduardo Guerra, Coah.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tiempo completo</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Postulación vía Indeed</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RECEPCIONISTA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>GAFI SERVICIOS SA DE CV</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Manufacturing Engr Manager</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Caterpillar</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Tiempo completo</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Indeed-Programador</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Supervisor, Production</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>YAZAKI Corporation</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Torreón, Coah.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>Indeed-Programador</t>
         </is>

</xml_diff>